<commit_message>
adapted sce tests for resonant grounding case
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/sce_tests/sc_result_comparison/wp_2.5/2_five_bus_radial_grid_dyn_gen_pf_sc_results_0_bus_resonant.xlsx
+++ b/pandapower/test/shortcircuit/sce_tests/sc_result_comparison/wp_2.5/2_five_bus_radial_grid_dyn_gen_pf_sc_results_0_bus_resonant.xlsx
@@ -719,40 +719,40 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.545454803106412</v>
+        <v>4.545454803106411</v>
       </c>
       <c r="D2">
-        <v>4.545454803106412</v>
+        <v>4.545454803106411</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>288.6751509579041</v>
+        <v>288.675150957904</v>
       </c>
       <c r="G2">
-        <v>288.6751509579041</v>
+        <v>288.675150957904</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
       </c>
       <c r="N2">
-        <v>0.9526279647803686</v>
+        <v>0.9526279647803685</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>0.9526279647833883</v>
       </c>
       <c r="Q2">
-        <v>-8.694577365250734E-11</v>
+        <v>-8.693806321708281E-11</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -811,16 +811,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9526279646671965</v>
+        <v>0.9526279646671958</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.9526279648965613</v>
+        <v>0.9526279648965605</v>
       </c>
       <c r="Q3">
-        <v>1.457296900362941E-10</v>
+        <v>1.457328738403161E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -870,22 +870,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9526279646404252</v>
+        <v>0.9526279646404247</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.9526279649233326</v>
+        <v>0.9526279649233319</v>
       </c>
       <c r="Q4">
-        <v>1.564846788178467E-09</v>
+        <v>1.564850104155587E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>179.9999999984264</v>
+        <v>179.9999999984265</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -929,16 +929,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9526279646315016</v>
+        <v>0.9526279646315009</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.9526279649322563</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q5">
-        <v>2.0378811364535E-09</v>
+        <v>2.037883569661619E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -988,16 +988,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9526279646315017</v>
+        <v>0.9526279646315008</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.9526279649322563</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q6">
-        <v>2.037882892602347E-09</v>
+        <v>2.037881073749259E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1101,19 +1101,19 @@
         <v>237.1508154128771</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
@@ -1122,16 +1122,16 @@
         <v>1.020226441408047</v>
       </c>
       <c r="O2">
-        <v>0.2400406982758469</v>
+        <v>0.2400406982758468</v>
       </c>
       <c r="P2">
         <v>0.8960735769153692</v>
       </c>
       <c r="Q2">
-        <v>5.766209884997121</v>
+        <v>5.766209884997131</v>
       </c>
       <c r="R2">
-        <v>-121.3466079962484</v>
+        <v>-121.3466079962483</v>
       </c>
       <c r="S2">
         <v>173.4315681772755</v>
@@ -1178,22 +1178,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.020226441315021</v>
+        <v>1.02022644131502</v>
       </c>
       <c r="O3">
-        <v>0.2400406981630192</v>
+        <v>0.2400406981630188</v>
       </c>
       <c r="P3">
-        <v>0.8960735770061727</v>
+        <v>0.8960735770061725</v>
       </c>
       <c r="Q3">
-        <v>5.766209884977167</v>
+        <v>5.766209884977173</v>
       </c>
       <c r="R3">
         <v>-121.3466079609365</v>
       </c>
       <c r="S3">
-        <v>173.4315681785683</v>
+        <v>173.4315681785684</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1237,22 +1237,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.020226441292308</v>
+        <v>1.020226441292307</v>
       </c>
       <c r="O4">
-        <v>0.2400406981651698</v>
+        <v>0.2400406981651691</v>
       </c>
       <c r="P4">
-        <v>0.8960735770323212</v>
+        <v>0.8960735770323207</v>
       </c>
       <c r="Q4">
-        <v>5.766209886018049</v>
+        <v>5.766209886018052</v>
       </c>
       <c r="R4">
-        <v>-121.3466079469511</v>
+        <v>-121.346607946951</v>
       </c>
       <c r="S4">
-        <v>173.4315681777208</v>
+        <v>173.4315681777209</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1296,22 +1296,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.020226441284737</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O5">
-        <v>0.2400406981658865</v>
+        <v>0.2400406981658859</v>
       </c>
       <c r="P5">
-        <v>0.8960735770410372</v>
+        <v>0.8960735770410369</v>
       </c>
       <c r="Q5">
-        <v>5.766209886365008</v>
+        <v>5.766209886365012</v>
       </c>
       <c r="R5">
         <v>-121.3466079422892</v>
       </c>
       <c r="S5">
-        <v>173.4315681774383</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1355,22 +1355,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.020226441284737</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O6">
-        <v>0.2400406981658865</v>
+        <v>0.240040698165886</v>
       </c>
       <c r="P6">
-        <v>0.8960735770410372</v>
+        <v>0.8960735770410369</v>
       </c>
       <c r="Q6">
-        <v>5.766209886365003</v>
+        <v>5.766209886365011</v>
       </c>
       <c r="R6">
-        <v>-121.3466079422893</v>
+        <v>-121.3466079422892</v>
       </c>
       <c r="S6">
-        <v>173.4315681774383</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
   </sheetData>
@@ -1468,19 +1468,19 @@
         <v>237.1508154128771</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
@@ -1489,16 +1489,16 @@
         <v>1.020226441408047</v>
       </c>
       <c r="O2">
-        <v>0.2400406982758469</v>
+        <v>0.2400406982758468</v>
       </c>
       <c r="P2">
         <v>0.8960735769153692</v>
       </c>
       <c r="Q2">
-        <v>5.766209884997121</v>
+        <v>5.766209884997131</v>
       </c>
       <c r="R2">
-        <v>-121.3466079962484</v>
+        <v>-121.3466079962483</v>
       </c>
       <c r="S2">
         <v>173.4315681772755</v>
@@ -1545,22 +1545,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.020226441315021</v>
+        <v>1.02022644131502</v>
       </c>
       <c r="O3">
-        <v>0.2400406981630192</v>
+        <v>0.2400406981630188</v>
       </c>
       <c r="P3">
-        <v>0.8960735770061727</v>
+        <v>0.8960735770061725</v>
       </c>
       <c r="Q3">
-        <v>5.766209884977167</v>
+        <v>5.766209884977173</v>
       </c>
       <c r="R3">
         <v>-121.3466079609365</v>
       </c>
       <c r="S3">
-        <v>173.4315681785683</v>
+        <v>173.4315681785684</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1604,22 +1604,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1.020226441292308</v>
+        <v>1.020226441292307</v>
       </c>
       <c r="O4">
-        <v>0.2400406981651698</v>
+        <v>0.2400406981651691</v>
       </c>
       <c r="P4">
-        <v>0.8960735770323212</v>
+        <v>0.8960735770323207</v>
       </c>
       <c r="Q4">
-        <v>5.766209886018049</v>
+        <v>5.766209886018052</v>
       </c>
       <c r="R4">
-        <v>-121.3466079469511</v>
+        <v>-121.346607946951</v>
       </c>
       <c r="S4">
-        <v>173.4315681777208</v>
+        <v>173.4315681777209</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1663,22 +1663,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>1.020226441284737</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O5">
-        <v>0.2400406981658865</v>
+        <v>0.2400406981658859</v>
       </c>
       <c r="P5">
-        <v>0.8960735770410372</v>
+        <v>0.8960735770410369</v>
       </c>
       <c r="Q5">
-        <v>5.766209886365008</v>
+        <v>5.766209886365012</v>
       </c>
       <c r="R5">
         <v>-121.3466079422892</v>
       </c>
       <c r="S5">
-        <v>173.4315681774383</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1722,22 +1722,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>1.020226441284737</v>
+        <v>1.020226441284736</v>
       </c>
       <c r="O6">
-        <v>0.2400406981658865</v>
+        <v>0.240040698165886</v>
       </c>
       <c r="P6">
-        <v>0.8960735770410372</v>
+        <v>0.8960735770410369</v>
       </c>
       <c r="Q6">
-        <v>5.766209886365003</v>
+        <v>5.766209886365011</v>
       </c>
       <c r="R6">
-        <v>-121.3466079422893</v>
+        <v>-121.3466079422892</v>
       </c>
       <c r="S6">
-        <v>173.4315681774383</v>
+        <v>173.4315681774384</v>
       </c>
     </row>
   </sheetData>
@@ -1820,19 +1820,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.63636376375428</v>
+        <v>3.636363763754283</v>
       </c>
       <c r="D2">
-        <v>3.63636376375428</v>
+        <v>3.636363763754283</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>230.9401157662428</v>
+        <v>230.940115766243</v>
       </c>
       <c r="G2">
-        <v>230.9401157662428</v>
+        <v>230.940115766243</v>
       </c>
       <c r="H2">
         <v>1.504993724976226</v>
@@ -1841,34 +1841,34 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
       </c>
       <c r="N2">
-        <v>0.8660254037845061</v>
+        <v>0.8660254037845059</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.86602540378499</v>
+        <v>0.8660254037849899</v>
       </c>
       <c r="Q2">
-        <v>1.720152468647288E-10</v>
+        <v>1.719944031106258E-10</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>179.9999999998193</v>
+        <v>179.9999999998194</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1912,16 +1912,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.8660254036789686</v>
+        <v>0.8660254036789684</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.8660254038905283</v>
+        <v>0.8660254038905281</v>
       </c>
       <c r="Q3">
-        <v>4.107386205101462E-10</v>
+        <v>4.107058638809503E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -1971,22 +1971,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.8660254036546317</v>
+        <v>0.8660254036546314</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.8660254039148658</v>
+        <v>0.8660254039148657</v>
       </c>
       <c r="Q4">
-        <v>3.1354257961412E-09</v>
+        <v>3.135402473591796E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>179.9999999968559</v>
+        <v>179.999999996856</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2030,16 +2030,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8660254036465191</v>
+        <v>0.8660254036465189</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.8660254039229784</v>
+        <v>0.8660254039229781</v>
       </c>
       <c r="Q5">
-        <v>4.043652235475932E-09</v>
+        <v>4.043635898052288E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8660254036465191</v>
+        <v>0.8660254036465189</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -2098,7 +2098,7 @@
         <v>0.8660254039229783</v>
       </c>
       <c r="Q6">
-        <v>4.043656440129865E-09</v>
+        <v>4.043634761181987E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2187,19 +2187,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.63636376375428</v>
+        <v>3.636363763754283</v>
       </c>
       <c r="D2">
-        <v>3.63636376375428</v>
+        <v>3.636363763754283</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>230.9401157662428</v>
+        <v>230.940115766243</v>
       </c>
       <c r="G2">
-        <v>230.9401157662428</v>
+        <v>230.940115766243</v>
       </c>
       <c r="H2">
         <v>1.504993724976226</v>
@@ -2208,34 +2208,34 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
       </c>
       <c r="N2">
-        <v>0.8660254037845061</v>
+        <v>0.8660254037845059</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.86602540378499</v>
+        <v>0.8660254037849899</v>
       </c>
       <c r="Q2">
-        <v>1.720152468647288E-10</v>
+        <v>1.719944031106258E-10</v>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
       <c r="S2">
-        <v>179.9999999998193</v>
+        <v>179.9999999998194</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2279,16 +2279,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.8660254036789686</v>
+        <v>0.8660254036789684</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.8660254038905283</v>
+        <v>0.8660254038905281</v>
       </c>
       <c r="Q3">
-        <v>4.107386205101462E-10</v>
+        <v>4.107058638809503E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -2338,22 +2338,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.8660254036546317</v>
+        <v>0.8660254036546314</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.8660254039148658</v>
+        <v>0.8660254039148657</v>
       </c>
       <c r="Q4">
-        <v>3.1354257961412E-09</v>
+        <v>3.135402473591796E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>179.9999999968559</v>
+        <v>179.999999996856</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2397,16 +2397,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8660254036465191</v>
+        <v>0.8660254036465189</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.8660254039229784</v>
+        <v>0.8660254039229781</v>
       </c>
       <c r="Q5">
-        <v>4.043652235475932E-09</v>
+        <v>4.043635898052288E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -2456,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8660254036465191</v>
+        <v>0.8660254036465189</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -2465,7 +2465,7 @@
         <v>0.8660254039229783</v>
       </c>
       <c r="Q6">
-        <v>4.043656440129865E-09</v>
+        <v>4.043634761181987E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2575,13 +2575,13 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -2593,7 +2593,7 @@
         <v>0.1964063473242863</v>
       </c>
       <c r="P2">
-        <v>0.8180121061818276</v>
+        <v>0.8180121061818275</v>
       </c>
       <c r="Q2">
         <v>5.173976904115775</v>
@@ -2646,19 +2646,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9220324943451758</v>
+        <v>0.9220324943451755</v>
       </c>
       <c r="O3">
-        <v>0.1964063472166729</v>
+        <v>0.1964063472166734</v>
       </c>
       <c r="P3">
-        <v>0.8180121062689192</v>
+        <v>0.8180121062689188</v>
       </c>
       <c r="Q3">
-        <v>5.173976904114568</v>
+        <v>5.173976904114571</v>
       </c>
       <c r="R3">
-        <v>-122.1449202549971</v>
+        <v>-122.144920254997</v>
       </c>
       <c r="S3">
         <v>174.1659345864976</v>
@@ -2708,19 +2708,19 @@
         <v>0.9220324943235492</v>
       </c>
       <c r="O4">
-        <v>0.1964063472443385</v>
+        <v>0.1964063472443389</v>
       </c>
       <c r="P4">
-        <v>0.8180121062966172</v>
+        <v>0.8180121062966171</v>
       </c>
       <c r="Q4">
-        <v>5.173976906219898</v>
+        <v>5.173976906219895</v>
       </c>
       <c r="R4">
         <v>-122.1449202329786</v>
       </c>
       <c r="S4">
-        <v>174.1659345844575</v>
+        <v>174.1659345844574</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -2764,16 +2764,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9220324943163404</v>
+        <v>0.9220324943163403</v>
       </c>
       <c r="O5">
-        <v>0.1964063472535603</v>
+        <v>0.1964063472535608</v>
       </c>
       <c r="P5">
-        <v>0.8180121063058501</v>
+        <v>0.8180121063058498</v>
       </c>
       <c r="Q5">
-        <v>5.173976906921674</v>
+        <v>5.173976906921673</v>
       </c>
       <c r="R5">
         <v>-122.1449202256391</v>
@@ -2823,16 +2823,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9220324943163404</v>
+        <v>0.9220324943163403</v>
       </c>
       <c r="O6">
-        <v>0.1964063472535603</v>
+        <v>0.1964063472535606</v>
       </c>
       <c r="P6">
-        <v>0.8180121063058501</v>
+        <v>0.8180121063058498</v>
       </c>
       <c r="Q6">
-        <v>5.173976906921678</v>
+        <v>5.173976906921672</v>
       </c>
       <c r="R6">
         <v>-122.1449202256391</v>
@@ -2942,13 +2942,13 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -2960,7 +2960,7 @@
         <v>0.1964063473242863</v>
       </c>
       <c r="P2">
-        <v>0.8180121061818276</v>
+        <v>0.8180121061818275</v>
       </c>
       <c r="Q2">
         <v>5.173976904115775</v>
@@ -3013,19 +3013,19 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9220324943451758</v>
+        <v>0.9220324943451755</v>
       </c>
       <c r="O3">
-        <v>0.1964063472166729</v>
+        <v>0.1964063472166734</v>
       </c>
       <c r="P3">
-        <v>0.8180121062689192</v>
+        <v>0.8180121062689188</v>
       </c>
       <c r="Q3">
-        <v>5.173976904114568</v>
+        <v>5.173976904114571</v>
       </c>
       <c r="R3">
-        <v>-122.1449202549971</v>
+        <v>-122.144920254997</v>
       </c>
       <c r="S3">
         <v>174.1659345864976</v>
@@ -3075,19 +3075,19 @@
         <v>0.9220324943235492</v>
       </c>
       <c r="O4">
-        <v>0.1964063472443385</v>
+        <v>0.1964063472443389</v>
       </c>
       <c r="P4">
-        <v>0.8180121062966172</v>
+        <v>0.8180121062966171</v>
       </c>
       <c r="Q4">
-        <v>5.173976906219898</v>
+        <v>5.173976906219895</v>
       </c>
       <c r="R4">
         <v>-122.1449202329786</v>
       </c>
       <c r="S4">
-        <v>174.1659345844575</v>
+        <v>174.1659345844574</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -3131,16 +3131,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9220324943163404</v>
+        <v>0.9220324943163403</v>
       </c>
       <c r="O5">
-        <v>0.1964063472535603</v>
+        <v>0.1964063472535608</v>
       </c>
       <c r="P5">
-        <v>0.8180121063058501</v>
+        <v>0.8180121063058498</v>
       </c>
       <c r="Q5">
-        <v>5.173976906921674</v>
+        <v>5.173976906921673</v>
       </c>
       <c r="R5">
         <v>-122.1449202256391</v>
@@ -3190,16 +3190,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9220324943163404</v>
+        <v>0.9220324943163403</v>
       </c>
       <c r="O6">
-        <v>0.1964063472535603</v>
+        <v>0.1964063472535606</v>
       </c>
       <c r="P6">
-        <v>0.8180121063058501</v>
+        <v>0.8180121063058498</v>
       </c>
       <c r="Q6">
-        <v>5.173976906921678</v>
+        <v>5.173976906921672</v>
       </c>
       <c r="R6">
         <v>-122.1449202256391</v>
@@ -3312,7 +3312,7 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163429</v>
+        <v>1.324394473163434</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
@@ -3330,16 +3330,16 @@
         <v>1.100000023884844</v>
       </c>
       <c r="P2">
-        <v>0.6350853099409384</v>
+        <v>0.6350853099409385</v>
       </c>
       <c r="Q2">
-        <v>59.99999999685335</v>
+        <v>59.99999999685337</v>
       </c>
       <c r="R2">
         <v>-89.99999999999635</v>
       </c>
       <c r="S2">
-        <v>119.9999999996536</v>
+        <v>119.9999999996535</v>
       </c>
       <c r="T2">
         <v>5.248639108526412</v>
@@ -3386,16 +3386,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6350853099894116</v>
+        <v>0.6350853099894119</v>
       </c>
       <c r="O3">
         <v>1.100000023884844</v>
       </c>
       <c r="P3">
-        <v>0.6350853098300097</v>
+        <v>0.63508530983001</v>
       </c>
       <c r="Q3">
-        <v>60.00000000239916</v>
+        <v>60.00000000239915</v>
       </c>
       <c r="R3">
         <v>-89.99999999999582</v>
@@ -3448,16 +3448,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853100298055</v>
+        <v>0.6350853100298057</v>
       </c>
       <c r="O4">
         <v>1.100000023884844</v>
       </c>
       <c r="P4">
-        <v>0.6350853098168608</v>
+        <v>0.6350853098168613</v>
       </c>
       <c r="Q4">
-        <v>60.00000000166492</v>
+        <v>60.0000000016649</v>
       </c>
       <c r="R4">
         <v>-89.99999999999582</v>
@@ -3510,16 +3510,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6350853100432702</v>
+        <v>0.6350853100432704</v>
       </c>
       <c r="O5">
         <v>1.100000023884844</v>
       </c>
       <c r="P5">
-        <v>0.6350853098124779</v>
+        <v>0.6350853098124783</v>
       </c>
       <c r="Q5">
-        <v>60.00000000142018</v>
+        <v>60.00000000142015</v>
       </c>
       <c r="R5">
         <v>-89.99999999999582</v>
@@ -3572,16 +3572,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6350853100432702</v>
+        <v>0.6350853100432704</v>
       </c>
       <c r="O6">
         <v>1.100000023884844</v>
       </c>
       <c r="P6">
-        <v>0.6350853098124778</v>
+        <v>0.6350853098124785</v>
       </c>
       <c r="Q6">
-        <v>60.00000000142018</v>
+        <v>60.00000000142015</v>
       </c>
       <c r="R6">
         <v>-89.99999999999582</v>
@@ -3697,7 +3697,7 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163429</v>
+        <v>1.324394473163434</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
@@ -3715,16 +3715,16 @@
         <v>1.100000023884844</v>
       </c>
       <c r="P2">
-        <v>0.6350853099409384</v>
+        <v>0.6350853099409385</v>
       </c>
       <c r="Q2">
-        <v>59.99999999685335</v>
+        <v>59.99999999685337</v>
       </c>
       <c r="R2">
         <v>-89.99999999999635</v>
       </c>
       <c r="S2">
-        <v>119.9999999996536</v>
+        <v>119.9999999996535</v>
       </c>
       <c r="T2">
         <v>5.248639108526412</v>
@@ -3771,16 +3771,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6350853099894116</v>
+        <v>0.6350853099894119</v>
       </c>
       <c r="O3">
         <v>1.100000023884844</v>
       </c>
       <c r="P3">
-        <v>0.6350853098300097</v>
+        <v>0.63508530983001</v>
       </c>
       <c r="Q3">
-        <v>60.00000000239916</v>
+        <v>60.00000000239915</v>
       </c>
       <c r="R3">
         <v>-89.99999999999582</v>
@@ -3833,16 +3833,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853100298055</v>
+        <v>0.6350853100298057</v>
       </c>
       <c r="O4">
         <v>1.100000023884844</v>
       </c>
       <c r="P4">
-        <v>0.6350853098168608</v>
+        <v>0.6350853098168613</v>
       </c>
       <c r="Q4">
-        <v>60.00000000166492</v>
+        <v>60.0000000016649</v>
       </c>
       <c r="R4">
         <v>-89.99999999999582</v>
@@ -3895,16 +3895,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6350853100432702</v>
+        <v>0.6350853100432704</v>
       </c>
       <c r="O5">
         <v>1.100000023884844</v>
       </c>
       <c r="P5">
-        <v>0.6350853098124779</v>
+        <v>0.6350853098124783</v>
       </c>
       <c r="Q5">
-        <v>60.00000000142018</v>
+        <v>60.00000000142015</v>
       </c>
       <c r="R5">
         <v>-89.99999999999582</v>
@@ -3957,16 +3957,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6350853100432702</v>
+        <v>0.6350853100432704</v>
       </c>
       <c r="O6">
         <v>1.100000023884844</v>
       </c>
       <c r="P6">
-        <v>0.6350853098124778</v>
+        <v>0.6350853098124785</v>
       </c>
       <c r="Q6">
-        <v>60.00000000142018</v>
+        <v>60.00000000142015</v>
       </c>
       <c r="R6">
         <v>-89.99999999999582</v>
@@ -4082,7 +4082,7 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163429</v>
+        <v>1.324394473163434</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
@@ -4094,7 +4094,7 @@
         <v>13.24394453563962</v>
       </c>
       <c r="N2">
-        <v>0.6918398877278028</v>
+        <v>0.6918398877278029</v>
       </c>
       <c r="O2">
         <v>1.100000023874158</v>
@@ -4162,7 +4162,7 @@
         <v>1.100000023874165</v>
       </c>
       <c r="P3">
-        <v>0.83784275781675</v>
+        <v>0.8378427578167501</v>
       </c>
       <c r="Q3">
         <v>40.40951796258041</v>
@@ -4171,7 +4171,7 @@
         <v>-89.99999999999615</v>
       </c>
       <c r="S3">
-        <v>128.9574716984651</v>
+        <v>128.9574716984652</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -4224,10 +4224,10 @@
         <v>1.100000023874165</v>
       </c>
       <c r="P4">
-        <v>0.8378427578056244</v>
+        <v>0.8378427578056247</v>
       </c>
       <c r="Q4">
-        <v>40.40951796344664</v>
+        <v>40.40951796344662</v>
       </c>
       <c r="R4">
         <v>-89.99999999999615</v>
@@ -4280,22 +4280,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6918398878066531</v>
+        <v>0.6918398878066532</v>
       </c>
       <c r="O5">
         <v>1.100000023874165</v>
       </c>
       <c r="P5">
-        <v>0.837842757801916</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q5">
-        <v>40.40951796373539</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R5">
         <v>-89.99999999999615</v>
       </c>
       <c r="S5">
-        <v>128.957471700848</v>
+        <v>128.9574717008481</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -4348,16 +4348,16 @@
         <v>1.100000023874165</v>
       </c>
       <c r="P6">
-        <v>0.837842757801916</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q6">
-        <v>40.4095179637354</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R6">
         <v>-89.99999999999615</v>
       </c>
       <c r="S6">
-        <v>128.957471700848</v>
+        <v>128.9574717008481</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -4618,7 +4618,7 @@
         <v>13.2439445349699</v>
       </c>
       <c r="J2">
-        <v>1.324394473163429</v>
+        <v>1.324394473163434</v>
       </c>
       <c r="K2">
         <v>13.24394453564036</v>
@@ -4630,7 +4630,7 @@
         <v>13.24394453563962</v>
       </c>
       <c r="N2">
-        <v>0.6918398877278028</v>
+        <v>0.6918398877278029</v>
       </c>
       <c r="O2">
         <v>1.100000023874158</v>
@@ -4698,7 +4698,7 @@
         <v>1.100000023874165</v>
       </c>
       <c r="P3">
-        <v>0.83784275781675</v>
+        <v>0.8378427578167501</v>
       </c>
       <c r="Q3">
         <v>40.40951796258041</v>
@@ -4707,7 +4707,7 @@
         <v>-89.99999999999615</v>
       </c>
       <c r="S3">
-        <v>128.9574716984651</v>
+        <v>128.9574716984652</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -4760,10 +4760,10 @@
         <v>1.100000023874165</v>
       </c>
       <c r="P4">
-        <v>0.8378427578056244</v>
+        <v>0.8378427578056247</v>
       </c>
       <c r="Q4">
-        <v>40.40951796344664</v>
+        <v>40.40951796344662</v>
       </c>
       <c r="R4">
         <v>-89.99999999999615</v>
@@ -4816,22 +4816,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.6918398878066531</v>
+        <v>0.6918398878066532</v>
       </c>
       <c r="O5">
         <v>1.100000023874165</v>
       </c>
       <c r="P5">
-        <v>0.837842757801916</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q5">
-        <v>40.40951796373539</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R5">
         <v>-89.99999999999615</v>
       </c>
       <c r="S5">
-        <v>128.957471700848</v>
+        <v>128.9574717008481</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -4884,16 +4884,16 @@
         <v>1.100000023874165</v>
       </c>
       <c r="P6">
-        <v>0.837842757801916</v>
+        <v>0.8378427578019162</v>
       </c>
       <c r="Q6">
-        <v>40.4095179637354</v>
+        <v>40.40951796373536</v>
       </c>
       <c r="R6">
         <v>-89.99999999999615</v>
       </c>
       <c r="S6">
-        <v>128.957471700848</v>
+        <v>128.9574717008481</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -4997,19 +4997,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976291</v>
+        <v>1.50499372497629</v>
       </c>
       <c r="I2">
         <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648793</v>
       </c>
       <c r="K2">
-        <v>15.04993697229388</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993720695425</v>
+        <v>1.504993720695426</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -5018,13 +5018,13 @@
         <v>0.5773502691155636</v>
       </c>
       <c r="O2">
-        <v>0.9999999999962956</v>
+        <v>0.9999999999962955</v>
       </c>
       <c r="P2">
-        <v>0.5773502692541785</v>
+        <v>0.5773502692541782</v>
       </c>
       <c r="Q2">
-        <v>59.99999999647621</v>
+        <v>59.99999999647622</v>
       </c>
       <c r="R2">
         <v>-89.99999999999635</v>
@@ -5080,13 +5080,13 @@
         <v>0.5773502692231756</v>
       </c>
       <c r="O3">
-        <v>0.9999999999962959</v>
+        <v>0.9999999999962957</v>
       </c>
       <c r="P3">
-        <v>0.5773502691507333</v>
+        <v>0.5773502691507328</v>
       </c>
       <c r="Q3">
-        <v>60.000000002165</v>
+        <v>60.00000000216502</v>
       </c>
       <c r="R3">
         <v>-89.99999999999582</v>
@@ -5145,10 +5145,10 @@
         <v>0.9999999999962959</v>
       </c>
       <c r="P4">
-        <v>0.5773502691501736</v>
+        <v>0.5773502691501732</v>
       </c>
       <c r="Q4">
-        <v>59.99999999947237</v>
+        <v>59.99999999947239</v>
       </c>
       <c r="R4">
         <v>-89.99999999999582</v>
@@ -5207,16 +5207,16 @@
         <v>0.9999999999962959</v>
       </c>
       <c r="P5">
-        <v>0.5773502691499868</v>
+        <v>0.5773502691499866</v>
       </c>
       <c r="Q5">
-        <v>59.99999999857482</v>
+        <v>59.99999999857485</v>
       </c>
       <c r="R5">
         <v>-89.99999999999582</v>
       </c>
       <c r="S5">
-        <v>120.0000000092881</v>
+        <v>120.000000009288</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -5269,16 +5269,16 @@
         <v>0.9999999999962959</v>
       </c>
       <c r="P6">
-        <v>0.5773502691499869</v>
+        <v>0.5773502691499866</v>
       </c>
       <c r="Q6">
-        <v>59.99999999857482</v>
+        <v>59.99999999857484</v>
       </c>
       <c r="R6">
         <v>-89.99999999999582</v>
       </c>
       <c r="S6">
-        <v>120.0000000092881</v>
+        <v>120.000000009288</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -5382,19 +5382,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976291</v>
+        <v>1.50499372497629</v>
       </c>
       <c r="I2">
         <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648793</v>
       </c>
       <c r="K2">
-        <v>15.04993697229388</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993720695425</v>
+        <v>1.504993720695426</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -5403,13 +5403,13 @@
         <v>0.5773502691155636</v>
       </c>
       <c r="O2">
-        <v>0.9999999999962956</v>
+        <v>0.9999999999962955</v>
       </c>
       <c r="P2">
-        <v>0.5773502692541785</v>
+        <v>0.5773502692541782</v>
       </c>
       <c r="Q2">
-        <v>59.99999999647621</v>
+        <v>59.99999999647622</v>
       </c>
       <c r="R2">
         <v>-89.99999999999635</v>
@@ -5465,13 +5465,13 @@
         <v>0.5773502692231756</v>
       </c>
       <c r="O3">
-        <v>0.9999999999962959</v>
+        <v>0.9999999999962957</v>
       </c>
       <c r="P3">
-        <v>0.5773502691507333</v>
+        <v>0.5773502691507328</v>
       </c>
       <c r="Q3">
-        <v>60.000000002165</v>
+        <v>60.00000000216502</v>
       </c>
       <c r="R3">
         <v>-89.99999999999582</v>
@@ -5530,10 +5530,10 @@
         <v>0.9999999999962959</v>
       </c>
       <c r="P4">
-        <v>0.5773502691501736</v>
+        <v>0.5773502691501732</v>
       </c>
       <c r="Q4">
-        <v>59.99999999947237</v>
+        <v>59.99999999947239</v>
       </c>
       <c r="R4">
         <v>-89.99999999999582</v>
@@ -5592,16 +5592,16 @@
         <v>0.9999999999962959</v>
       </c>
       <c r="P5">
-        <v>0.5773502691499868</v>
+        <v>0.5773502691499866</v>
       </c>
       <c r="Q5">
-        <v>59.99999999857482</v>
+        <v>59.99999999857485</v>
       </c>
       <c r="R5">
         <v>-89.99999999999582</v>
       </c>
       <c r="S5">
-        <v>120.0000000092881</v>
+        <v>120.000000009288</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -5654,16 +5654,16 @@
         <v>0.9999999999962959</v>
       </c>
       <c r="P6">
-        <v>0.5773502691499869</v>
+        <v>0.5773502691499866</v>
       </c>
       <c r="Q6">
-        <v>59.99999999857482</v>
+        <v>59.99999999857484</v>
       </c>
       <c r="R6">
         <v>-89.99999999999582</v>
       </c>
       <c r="S6">
-        <v>120.0000000092881</v>
+        <v>120.000000009288</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -5767,19 +5767,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976291</v>
+        <v>1.50499372497629</v>
       </c>
       <c r="I2">
         <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648793</v>
       </c>
       <c r="K2">
-        <v>15.04993697229388</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993720695425</v>
+        <v>1.504993720695426</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -5788,7 +5788,7 @@
         <v>0.6184267549947473</v>
       </c>
       <c r="O2">
-        <v>0.9999999999908645</v>
+        <v>0.9999999999908644</v>
       </c>
       <c r="P2">
         <v>0.747299752735181</v>
@@ -5850,16 +5850,16 @@
         <v>0.6184267550404209</v>
       </c>
       <c r="O3">
-        <v>0.999999999990871</v>
+        <v>0.9999999999908711</v>
       </c>
       <c r="P3">
-        <v>0.7472997526577984</v>
+        <v>0.7472997526577982</v>
       </c>
       <c r="Q3">
         <v>41.77463363810636</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999612</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S3">
         <v>128.1091583228107</v>
@@ -5915,16 +5915,16 @@
         <v>0.9999999999908711</v>
       </c>
       <c r="P4">
-        <v>0.7472997526545259</v>
+        <v>0.7472997526545258</v>
       </c>
       <c r="Q4">
-        <v>41.77463363817495</v>
+        <v>41.77463363817496</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999612</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S4">
-        <v>128.1091583258393</v>
+        <v>128.1091583258392</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -5980,7 +5980,7 @@
         <v>0.747299752653435</v>
       </c>
       <c r="Q5">
-        <v>41.77463363819783</v>
+        <v>41.77463363819784</v>
       </c>
       <c r="R5">
         <v>-89.99999999999613</v>
@@ -6033,19 +6033,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6184267550932595</v>
+        <v>0.6184267550932593</v>
       </c>
       <c r="O6">
         <v>0.9999999999908711</v>
       </c>
       <c r="P6">
-        <v>0.7472997526534351</v>
+        <v>0.747299752653435</v>
       </c>
       <c r="Q6">
-        <v>41.77463363819783</v>
+        <v>41.77463363819785</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999613</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S6">
         <v>128.1091583268488</v>
@@ -6152,19 +6152,19 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1.504993724976291</v>
+        <v>1.50499372497629</v>
       </c>
       <c r="I2">
         <v>15.04993697142823</v>
       </c>
       <c r="J2">
-        <v>1.504993722648794</v>
+        <v>1.504993722648793</v>
       </c>
       <c r="K2">
-        <v>15.04993697229388</v>
+        <v>15.04993697229387</v>
       </c>
       <c r="L2">
-        <v>1.504993720695425</v>
+        <v>1.504993720695426</v>
       </c>
       <c r="M2">
         <v>15.04993697229304</v>
@@ -6173,7 +6173,7 @@
         <v>0.6184267549947473</v>
       </c>
       <c r="O2">
-        <v>0.9999999999908645</v>
+        <v>0.9999999999908644</v>
       </c>
       <c r="P2">
         <v>0.747299752735181</v>
@@ -6235,16 +6235,16 @@
         <v>0.6184267550404209</v>
       </c>
       <c r="O3">
-        <v>0.999999999990871</v>
+        <v>0.9999999999908711</v>
       </c>
       <c r="P3">
-        <v>0.7472997526577984</v>
+        <v>0.7472997526577982</v>
       </c>
       <c r="Q3">
         <v>41.77463363810636</v>
       </c>
       <c r="R3">
-        <v>-89.99999999999612</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S3">
         <v>128.1091583228107</v>
@@ -6300,16 +6300,16 @@
         <v>0.9999999999908711</v>
       </c>
       <c r="P4">
-        <v>0.7472997526545259</v>
+        <v>0.7472997526545258</v>
       </c>
       <c r="Q4">
-        <v>41.77463363817495</v>
+        <v>41.77463363817496</v>
       </c>
       <c r="R4">
-        <v>-89.99999999999612</v>
+        <v>-89.99999999999613</v>
       </c>
       <c r="S4">
-        <v>128.1091583258393</v>
+        <v>128.1091583258392</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -6365,7 +6365,7 @@
         <v>0.747299752653435</v>
       </c>
       <c r="Q5">
-        <v>41.77463363819783</v>
+        <v>41.77463363819784</v>
       </c>
       <c r="R5">
         <v>-89.99999999999613</v>
@@ -6418,19 +6418,19 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6184267550932595</v>
+        <v>0.6184267550932593</v>
       </c>
       <c r="O6">
         <v>0.9999999999908711</v>
       </c>
       <c r="P6">
-        <v>0.7472997526534351</v>
+        <v>0.747299752653435</v>
       </c>
       <c r="Q6">
-        <v>41.77463363819783</v>
+        <v>41.77463363819785</v>
       </c>
       <c r="R6">
-        <v>-89.99999999999613</v>
+        <v>-89.99999999999615</v>
       </c>
       <c r="S6">
         <v>128.1091583268488</v>
@@ -6522,49 +6522,49 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5.24863910873685</v>
+        <v>5.248639108736849</v>
       </c>
       <c r="D2">
-        <v>5.248639107970815</v>
+        <v>5.248639107970814</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>333.333352253926</v>
+        <v>333.3333522539259</v>
       </c>
       <c r="G2">
         <v>333.3333522052762</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
       </c>
       <c r="N2">
-        <v>0.6350853098347086</v>
+        <v>0.6350853098347087</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6350853098507082</v>
+        <v>0.6350853098507081</v>
       </c>
       <c r="Q2">
-        <v>-4.877407190948084E-09</v>
+        <v>-4.877405252462882E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -6573,7 +6573,7 @@
         <v>179.999999996043</v>
       </c>
       <c r="T2">
-        <v>5.248639108420278</v>
+        <v>5.248639108420277</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -6623,16 +6623,16 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.6350853099661095</v>
+        <v>0.6350853099661091</v>
       </c>
       <c r="Q3">
-        <v>1.367218423137133E-09</v>
+        <v>1.36725217887024E-09</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3">
-        <v>-179.9999999983959</v>
+        <v>-179.9999999983958</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -6679,16 +6679,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853097106263</v>
+        <v>0.635085309710626</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.6350853100065034</v>
+        <v>0.635085310006503</v>
       </c>
       <c r="Q4">
-        <v>4.890337327767773E-09</v>
+        <v>4.890364378988421E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -6747,16 +6747,16 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.6350853100199679</v>
+        <v>0.6350853100199676</v>
       </c>
       <c r="Q5">
-        <v>6.064693964128537E-09</v>
+        <v>6.064726305644647E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>-179.9999999993749</v>
+        <v>-179.9999999993748</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -6803,22 +6803,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6350853097062433</v>
+        <v>0.6350853097062432</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.6350853100199679</v>
+        <v>0.6350853100199676</v>
       </c>
       <c r="Q6">
-        <v>6.064698971729444E-09</v>
+        <v>6.064721634335353E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>-179.9999999993749</v>
+        <v>-179.9999999993748</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -6907,49 +6907,49 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5.24863910873685</v>
+        <v>5.248639108736849</v>
       </c>
       <c r="D2">
-        <v>5.248639107970815</v>
+        <v>5.248639107970814</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>333.333352253926</v>
+        <v>333.3333522539259</v>
       </c>
       <c r="G2">
         <v>333.3333522052762</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
       </c>
       <c r="N2">
-        <v>0.6350853098347086</v>
+        <v>0.6350853098347087</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.6350853098507082</v>
+        <v>0.6350853098507081</v>
       </c>
       <c r="Q2">
-        <v>-4.877407190948084E-09</v>
+        <v>-4.877405252462882E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -6958,7 +6958,7 @@
         <v>179.999999996043</v>
       </c>
       <c r="T2">
-        <v>5.248639108420278</v>
+        <v>5.248639108420277</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -7008,16 +7008,16 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.6350853099661095</v>
+        <v>0.6350853099661091</v>
       </c>
       <c r="Q3">
-        <v>1.367218423137133E-09</v>
+        <v>1.36725217887024E-09</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3">
-        <v>-179.9999999983959</v>
+        <v>-179.9999999983958</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -7064,16 +7064,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.6350853097106263</v>
+        <v>0.635085309710626</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.6350853100065034</v>
+        <v>0.635085310006503</v>
       </c>
       <c r="Q4">
-        <v>4.890337327767773E-09</v>
+        <v>4.890364378988421E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -7132,16 +7132,16 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.6350853100199679</v>
+        <v>0.6350853100199676</v>
       </c>
       <c r="Q5">
-        <v>6.064693964128537E-09</v>
+        <v>6.064726305644647E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>-179.9999999993749</v>
+        <v>-179.9999999993748</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -7188,22 +7188,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6350853097062433</v>
+        <v>0.6350853097062432</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.6350853100199679</v>
+        <v>0.6350853100199676</v>
       </c>
       <c r="Q6">
-        <v>6.064698971729444E-09</v>
+        <v>6.064721634335353E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>-179.9999999993749</v>
+        <v>-179.9999999993748</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -7295,7 +7295,7 @@
         <v>3.617960382593723</v>
       </c>
       <c r="D2">
-        <v>3.617960382231207</v>
+        <v>3.617960382231205</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -7307,19 +7307,19 @@
         <v>229.7713440658447</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
@@ -7331,7 +7331,7 @@
         <v>0.4028253111898906</v>
       </c>
       <c r="P2">
-        <v>0.6918398877011798</v>
+        <v>0.6918398877011797</v>
       </c>
       <c r="Q2">
         <v>8.957471693504779</v>
@@ -7343,7 +7343,7 @@
         <v>160.4095179569557</v>
       </c>
       <c r="T2">
-        <v>3.617960382370079</v>
+        <v>3.617960382370078</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -7387,16 +7387,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.837842757745752</v>
+        <v>0.8378427577457516</v>
       </c>
       <c r="O3">
-        <v>0.4028253110952159</v>
+        <v>0.4028253110952154</v>
       </c>
       <c r="P3">
-        <v>0.6918398877448092</v>
+        <v>0.6918398877448086</v>
       </c>
       <c r="Q3">
-        <v>8.95747169635165</v>
+        <v>8.957471696351648</v>
       </c>
       <c r="R3">
         <v>-115.8807585788046</v>
@@ -7449,22 +7449,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.8378427577346269</v>
+        <v>0.8378427577346264</v>
       </c>
       <c r="O4">
-        <v>0.4028253110970205</v>
+        <v>0.40282531109702</v>
       </c>
       <c r="P4">
-        <v>0.6918398877712167</v>
+        <v>0.6918398877712163</v>
       </c>
       <c r="Q4">
-        <v>8.95747169813882</v>
+        <v>8.957471698138814</v>
       </c>
       <c r="R4">
         <v>-115.8807585718119</v>
       </c>
       <c r="S4">
-        <v>160.4095179643535</v>
+        <v>160.4095179643536</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -7511,19 +7511,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8378427577309184</v>
+        <v>0.8378427577309179</v>
       </c>
       <c r="O5">
-        <v>0.402825311097622</v>
+        <v>0.4028253110976214</v>
       </c>
       <c r="P5">
-        <v>0.6918398877800191</v>
+        <v>0.6918398877800188</v>
       </c>
       <c r="Q5">
-        <v>8.957471698734537</v>
+        <v>8.957471698734539</v>
       </c>
       <c r="R5">
-        <v>-115.880758569481</v>
+        <v>-115.8807585694809</v>
       </c>
       <c r="S5">
         <v>160.4095179646423</v>
@@ -7573,16 +7573,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8378427577309184</v>
+        <v>0.8378427577309178</v>
       </c>
       <c r="O6">
-        <v>0.402825311097622</v>
+        <v>0.4028253110976213</v>
       </c>
       <c r="P6">
-        <v>0.6918398877800191</v>
+        <v>0.6918398877800188</v>
       </c>
       <c r="Q6">
-        <v>8.95747169873454</v>
+        <v>8.957471698734535</v>
       </c>
       <c r="R6">
         <v>-115.880758569481</v>
@@ -7680,7 +7680,7 @@
         <v>3.617960382593723</v>
       </c>
       <c r="D2">
-        <v>3.617960382231207</v>
+        <v>3.617960382231205</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -7692,19 +7692,19 @@
         <v>229.7713440658447</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
@@ -7716,7 +7716,7 @@
         <v>0.4028253111898906</v>
       </c>
       <c r="P2">
-        <v>0.6918398877011798</v>
+        <v>0.6918398877011797</v>
       </c>
       <c r="Q2">
         <v>8.957471693504779</v>
@@ -7728,7 +7728,7 @@
         <v>160.4095179569557</v>
       </c>
       <c r="T2">
-        <v>3.617960382370079</v>
+        <v>3.617960382370078</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -7772,16 +7772,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.837842757745752</v>
+        <v>0.8378427577457516</v>
       </c>
       <c r="O3">
-        <v>0.4028253110952159</v>
+        <v>0.4028253110952154</v>
       </c>
       <c r="P3">
-        <v>0.6918398877448092</v>
+        <v>0.6918398877448086</v>
       </c>
       <c r="Q3">
-        <v>8.95747169635165</v>
+        <v>8.957471696351648</v>
       </c>
       <c r="R3">
         <v>-115.8807585788046</v>
@@ -7834,22 +7834,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.8378427577346269</v>
+        <v>0.8378427577346264</v>
       </c>
       <c r="O4">
-        <v>0.4028253110970205</v>
+        <v>0.40282531109702</v>
       </c>
       <c r="P4">
-        <v>0.6918398877712167</v>
+        <v>0.6918398877712163</v>
       </c>
       <c r="Q4">
-        <v>8.95747169813882</v>
+        <v>8.957471698138814</v>
       </c>
       <c r="R4">
         <v>-115.8807585718119</v>
       </c>
       <c r="S4">
-        <v>160.4095179643535</v>
+        <v>160.4095179643536</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -7896,19 +7896,19 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.8378427577309184</v>
+        <v>0.8378427577309179</v>
       </c>
       <c r="O5">
-        <v>0.402825311097622</v>
+        <v>0.4028253110976214</v>
       </c>
       <c r="P5">
-        <v>0.6918398877800191</v>
+        <v>0.6918398877800188</v>
       </c>
       <c r="Q5">
-        <v>8.957471698734537</v>
+        <v>8.957471698734539</v>
       </c>
       <c r="R5">
-        <v>-115.880758569481</v>
+        <v>-115.8807585694809</v>
       </c>
       <c r="S5">
         <v>160.4095179646423</v>
@@ -7958,16 +7958,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.8378427577309184</v>
+        <v>0.8378427577309178</v>
       </c>
       <c r="O6">
-        <v>0.402825311097622</v>
+        <v>0.4028253110976213</v>
       </c>
       <c r="P6">
-        <v>0.6918398877800191</v>
+        <v>0.6918398877800188</v>
       </c>
       <c r="Q6">
-        <v>8.95747169873454</v>
+        <v>8.957471698734535</v>
       </c>
       <c r="R6">
         <v>-115.880758569481</v>
@@ -8065,7 +8065,7 @@
         <v>4.198911196109218</v>
       </c>
       <c r="D2">
-        <v>4.198911195412806</v>
+        <v>4.198911195412807</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -8083,28 +8083,28 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
       </c>
       <c r="N2">
-        <v>0.5773502691952341</v>
+        <v>0.577350269195234</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5773502691743767</v>
+        <v>0.5773502691743763</v>
       </c>
       <c r="Q2">
-        <v>-5.812893200252229E-09</v>
+        <v>-5.812908622049256E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -8113,7 +8113,7 @@
         <v>179.9999999936331</v>
       </c>
       <c r="T2">
-        <v>4.198911195821409</v>
+        <v>4.19891119582141</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -8157,16 +8157,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.5773502690917846</v>
+        <v>0.5773502690917844</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.5773502692819935</v>
+        <v>0.5773502692819928</v>
       </c>
       <c r="Q3">
-        <v>5.928560750305164E-10</v>
+        <v>5.928262743863529E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -8219,16 +8219,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.5773502690912251</v>
+        <v>0.5773502690912249</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.5773502693301086</v>
+        <v>0.5773502693301079</v>
       </c>
       <c r="Q4">
-        <v>6.074310315194379E-09</v>
+        <v>6.074293935282762E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -8281,22 +8281,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.5773502690910385</v>
+        <v>0.5773502690910384</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.5773502693461469</v>
+        <v>0.5773502693461464</v>
       </c>
       <c r="Q5">
-        <v>7.901472358927767E-09</v>
+        <v>7.901452798975248E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -8343,22 +8343,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.5773502690910385</v>
+        <v>0.5773502690910384</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.5773502693461469</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q6">
-        <v>7.901473002427768E-09</v>
+        <v>7.901456249486592E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -8601,7 +8601,7 @@
         <v>4.198911196109218</v>
       </c>
       <c r="D2">
-        <v>4.198911195412806</v>
+        <v>4.198911195412807</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -8619,28 +8619,28 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
       </c>
       <c r="N2">
-        <v>0.5773502691952341</v>
+        <v>0.577350269195234</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0.5773502691743767</v>
+        <v>0.5773502691743763</v>
       </c>
       <c r="Q2">
-        <v>-5.812893200252229E-09</v>
+        <v>-5.812908622049256E-09</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -8649,7 +8649,7 @@
         <v>179.9999999936331</v>
       </c>
       <c r="T2">
-        <v>4.198911195821409</v>
+        <v>4.19891119582141</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -8693,16 +8693,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.5773502690917846</v>
+        <v>0.5773502690917844</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.5773502692819935</v>
+        <v>0.5773502692819928</v>
       </c>
       <c r="Q3">
-        <v>5.928560750305164E-10</v>
+        <v>5.928262743863529E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -8755,16 +8755,16 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.5773502690912251</v>
+        <v>0.5773502690912249</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.5773502693301086</v>
+        <v>0.5773502693301079</v>
       </c>
       <c r="Q4">
-        <v>6.074310315194379E-09</v>
+        <v>6.074293935282762E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -8817,22 +8817,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.5773502690910385</v>
+        <v>0.5773502690910384</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.5773502693461469</v>
+        <v>0.5773502693461464</v>
       </c>
       <c r="Q5">
-        <v>7.901472358927767E-09</v>
+        <v>7.901452798975248E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
       </c>
       <c r="S5">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -8879,22 +8879,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.5773502690910385</v>
+        <v>0.5773502690910384</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.5773502693461469</v>
+        <v>0.5773502693461462</v>
       </c>
       <c r="Q6">
-        <v>7.901473002427768E-09</v>
+        <v>7.901456249486592E-09</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>179.9999999957326</v>
+        <v>179.9999999957325</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -8983,16 +8983,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.012913138951924</v>
+        <v>3.012913138951925</v>
       </c>
       <c r="D2">
-        <v>3.012913138593917</v>
+        <v>3.012913138593918</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>191.3456833000739</v>
+        <v>191.345683300074</v>
       </c>
       <c r="G2">
         <v>191.3456832773375</v>
@@ -9004,13 +9004,13 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -9019,22 +9019,22 @@
         <v>0.7472997527192564</v>
       </c>
       <c r="O2">
-        <v>0.3354590831689601</v>
+        <v>0.3354590831689602</v>
       </c>
       <c r="P2">
-        <v>0.6184267550384417</v>
+        <v>0.6184267550384414</v>
       </c>
       <c r="Q2">
         <v>8.109158318802281</v>
       </c>
       <c r="R2">
-        <v>-117.0248837767961</v>
+        <v>-117.0248837767962</v>
       </c>
       <c r="S2">
         <v>161.7746336318227</v>
       </c>
       <c r="T2">
-        <v>3.012913138737344</v>
+        <v>3.012913138737345</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -9078,22 +9078,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.747299752641862</v>
+        <v>0.7472997526418619</v>
       </c>
       <c r="O3">
-        <v>0.3354590830770567</v>
+        <v>0.3354590830770568</v>
       </c>
       <c r="P3">
-        <v>0.6184267550841063</v>
+        <v>0.6184267550841056</v>
       </c>
       <c r="Q3">
-        <v>8.109158321931368</v>
+        <v>8.109158321931361</v>
       </c>
       <c r="R3">
         <v>-117.0248837562166</v>
       </c>
       <c r="S3">
-        <v>161.7746336387373</v>
+        <v>161.7746336387372</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -9140,19 +9140,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.7472997526385897</v>
+        <v>0.7472997526385895</v>
       </c>
       <c r="O4">
-        <v>0.3354590831006828</v>
+        <v>0.335459083100683</v>
       </c>
       <c r="P4">
-        <v>0.6184267551237351</v>
+        <v>0.6184267551237346</v>
       </c>
       <c r="Q4">
-        <v>8.109158324959862</v>
+        <v>8.109158324959855</v>
       </c>
       <c r="R4">
-        <v>-117.0248837452073</v>
+        <v>-117.0248837452074</v>
       </c>
       <c r="S4">
         <v>161.7746336388059</v>
@@ -9202,22 +9202,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.7472997526374988</v>
+        <v>0.7472997526374987</v>
       </c>
       <c r="O5">
-        <v>0.3354590831085582</v>
+        <v>0.3354590831085584</v>
       </c>
       <c r="P5">
-        <v>0.6184267551369448</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q5">
-        <v>8.109158325969364</v>
+        <v>8.109158325969359</v>
       </c>
       <c r="R5">
-        <v>-117.0248837415376</v>
+        <v>-117.0248837415377</v>
       </c>
       <c r="S5">
-        <v>161.7746336388288</v>
+        <v>161.7746336388287</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -9264,22 +9264,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.7472997526374988</v>
+        <v>0.7472997526374985</v>
       </c>
       <c r="O6">
-        <v>0.3354590831085583</v>
+        <v>0.3354590831085584</v>
       </c>
       <c r="P6">
-        <v>0.6184267551369447</v>
+        <v>0.6184267551369441</v>
       </c>
       <c r="Q6">
-        <v>8.109158325969371</v>
+        <v>8.109158325969355</v>
       </c>
       <c r="R6">
-        <v>-117.0248837415376</v>
+        <v>-117.0248837415377</v>
       </c>
       <c r="S6">
-        <v>161.7746336388288</v>
+        <v>161.7746336388287</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -9368,16 +9368,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>3.012913138951924</v>
+        <v>3.012913138951925</v>
       </c>
       <c r="D2">
-        <v>3.012913138593917</v>
+        <v>3.012913138593918</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>191.3456833000739</v>
+        <v>191.345683300074</v>
       </c>
       <c r="G2">
         <v>191.3456832773375</v>
@@ -9389,13 +9389,13 @@
         <v>15.04993697142947</v>
       </c>
       <c r="J2">
-        <v>1.504993721246239</v>
+        <v>1.504993721246244</v>
       </c>
       <c r="K2">
         <v>15.04993697324838</v>
       </c>
       <c r="L2">
-        <v>1.504993720695297</v>
+        <v>1.5049937206953</v>
       </c>
       <c r="M2">
         <v>15.04993697229334</v>
@@ -9404,22 +9404,22 @@
         <v>0.7472997527192564</v>
       </c>
       <c r="O2">
-        <v>0.3354590831689601</v>
+        <v>0.3354590831689602</v>
       </c>
       <c r="P2">
-        <v>0.6184267550384417</v>
+        <v>0.6184267550384414</v>
       </c>
       <c r="Q2">
         <v>8.109158318802281</v>
       </c>
       <c r="R2">
-        <v>-117.0248837767961</v>
+        <v>-117.0248837767962</v>
       </c>
       <c r="S2">
         <v>161.7746336318227</v>
       </c>
       <c r="T2">
-        <v>3.012913138737344</v>
+        <v>3.012913138737345</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -9463,22 +9463,22 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.747299752641862</v>
+        <v>0.7472997526418619</v>
       </c>
       <c r="O3">
-        <v>0.3354590830770567</v>
+        <v>0.3354590830770568</v>
       </c>
       <c r="P3">
-        <v>0.6184267550841063</v>
+        <v>0.6184267550841056</v>
       </c>
       <c r="Q3">
-        <v>8.109158321931368</v>
+        <v>8.109158321931361</v>
       </c>
       <c r="R3">
         <v>-117.0248837562166</v>
       </c>
       <c r="S3">
-        <v>161.7746336387373</v>
+        <v>161.7746336387372</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -9525,19 +9525,19 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.7472997526385897</v>
+        <v>0.7472997526385895</v>
       </c>
       <c r="O4">
-        <v>0.3354590831006828</v>
+        <v>0.335459083100683</v>
       </c>
       <c r="P4">
-        <v>0.6184267551237351</v>
+        <v>0.6184267551237346</v>
       </c>
       <c r="Q4">
-        <v>8.109158324959862</v>
+        <v>8.109158324959855</v>
       </c>
       <c r="R4">
-        <v>-117.0248837452073</v>
+        <v>-117.0248837452074</v>
       </c>
       <c r="S4">
         <v>161.7746336388059</v>
@@ -9587,22 +9587,22 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.7472997526374988</v>
+        <v>0.7472997526374987</v>
       </c>
       <c r="O5">
-        <v>0.3354590831085582</v>
+        <v>0.3354590831085584</v>
       </c>
       <c r="P5">
-        <v>0.6184267551369448</v>
+        <v>0.6184267551369443</v>
       </c>
       <c r="Q5">
-        <v>8.109158325969364</v>
+        <v>8.109158325969359</v>
       </c>
       <c r="R5">
-        <v>-117.0248837415376</v>
+        <v>-117.0248837415377</v>
       </c>
       <c r="S5">
-        <v>161.7746336388288</v>
+        <v>161.7746336388287</v>
       </c>
       <c r="T5">
         <v>0</v>
@@ -9649,22 +9649,22 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.7472997526374988</v>
+        <v>0.7472997526374985</v>
       </c>
       <c r="O6">
-        <v>0.3354590831085583</v>
+        <v>0.3354590831085584</v>
       </c>
       <c r="P6">
-        <v>0.6184267551369447</v>
+        <v>0.6184267551369441</v>
       </c>
       <c r="Q6">
-        <v>8.109158325969371</v>
+        <v>8.109158325969355</v>
       </c>
       <c r="R6">
-        <v>-117.0248837415376</v>
+        <v>-117.0248837415377</v>
       </c>
       <c r="S6">
-        <v>161.7746336388288</v>
+        <v>161.7746336388287</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -10505,40 +10505,40 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>4.545454803106412</v>
+        <v>4.545454803106411</v>
       </c>
       <c r="D2">
-        <v>4.545454803106412</v>
+        <v>4.545454803106411</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>288.6751509579041</v>
+        <v>288.675150957904</v>
       </c>
       <c r="G2">
-        <v>288.6751509579041</v>
+        <v>288.675150957904</v>
       </c>
       <c r="H2">
-        <v>1.324394477419386</v>
+        <v>1.324394477419385</v>
       </c>
       <c r="I2">
-        <v>13.24394453497101</v>
+        <v>13.243944534971</v>
       </c>
       <c r="J2">
-        <v>1.324394474186049</v>
+        <v>1.324394474186053</v>
       </c>
       <c r="K2">
         <v>13.24394453578229</v>
       </c>
       <c r="L2">
-        <v>1.324394474104232</v>
+        <v>1.32439447410423</v>
       </c>
       <c r="M2">
         <v>13.24394453563989</v>
       </c>
       <c r="N2">
-        <v>0.9526279647803686</v>
+        <v>0.9526279647803685</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -10547,7 +10547,7 @@
         <v>0.9526279647833883</v>
       </c>
       <c r="Q2">
-        <v>-8.694577365250734E-11</v>
+        <v>-8.693806321708281E-11</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -10597,16 +10597,16 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.9526279646671965</v>
+        <v>0.9526279646671958</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.9526279648965613</v>
+        <v>0.9526279648965605</v>
       </c>
       <c r="Q3">
-        <v>1.457296900362941E-10</v>
+        <v>1.457328738403161E-10</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -10656,22 +10656,22 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.9526279646404252</v>
+        <v>0.9526279646404247</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0.9526279649233326</v>
+        <v>0.9526279649233319</v>
       </c>
       <c r="Q4">
-        <v>1.564846788178467E-09</v>
+        <v>1.564850104155587E-09</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4">
-        <v>179.9999999984264</v>
+        <v>179.9999999984265</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -10715,16 +10715,16 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.9526279646315016</v>
+        <v>0.9526279646315009</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0.9526279649322563</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q5">
-        <v>2.0378811364535E-09</v>
+        <v>2.037883569661619E-09</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -10774,16 +10774,16 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.9526279646315017</v>
+        <v>0.9526279646315008</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0.9526279649322563</v>
+        <v>0.9526279649322557</v>
       </c>
       <c r="Q6">
-        <v>2.037882892602347E-09</v>
+        <v>2.037881073749259E-09</v>
       </c>
       <c r="R6">
         <v>0</v>

</xml_diff>